<commit_message>
Add offline attendance system with ST7789 display support and WiFi auto-detection
</commit_message>
<xml_diff>
--- a/data/attendance.xlsx
+++ b/data/attendance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Attendance" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Monthly Report" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Attendance" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Monthly Report" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -446,13 +446,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
@@ -826,6 +826,80 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Linh</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>09:18:51</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>LATE</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>1h 18m</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>bb</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>11:24:40</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>11:34:34</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0h 9m</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>LATE</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>3h 24m</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0m</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -837,13 +911,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
@@ -928,30 +1002,30 @@
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
         <is>
-          <t>TestUser2</t>
+          <t>Linh</t>
         </is>
       </c>
       <c r="B4" s="4" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t>11h 13m</t>
+          <t>1h 18m</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t>13m</t>
+          <t>0m</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>TestUser3</t>
+          <t>TestUser2</t>
         </is>
       </c>
       <c r="B5" s="4" t="n">
@@ -962,19 +1036,19 @@
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t>11h 19m</t>
+          <t>11h 13m</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t>19m</t>
+          <t>13m</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>User1</t>
+          <t>TestUser3</t>
         </is>
       </c>
       <c r="B6" s="4" t="n">
@@ -985,33 +1059,79 @@
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t>11h 22m</t>
+          <t>11h 19m</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t>22m</t>
+          <t>19m</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
+          <t>User1</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>11h 22m</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>22m</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>bb</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>3h 24m</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="inlineStr">
+        <is>
           <t>gg</t>
         </is>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="n">
+      <c r="B9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="4" t="inlineStr">
+      <c r="D9" s="4" t="inlineStr">
         <is>
           <t>11h 16m</t>
         </is>
       </c>
-      <c r="E7" s="4" t="inlineStr">
+      <c r="E9" s="4" t="inlineStr">
         <is>
           <t>8h 57m</t>
         </is>

</xml_diff>